<commit_message>
Added lightning talk from Alchemy Code Lab Students for Feb. 2020.
</commit_message>
<xml_diff>
--- a/talks/Upcoming Speaker Schedule/pdx-node-speaker-schedule.xlsx
+++ b/talks/Upcoming Speaker Schedule/pdx-node-speaker-schedule.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="10">
   <si>
     <t>PDX Node Upcoming Speaker Schedule</t>
   </si>
@@ -19,29 +19,13 @@
     <t>Month</t>
   </si>
   <si>
-    <t>Speaker</t>
+    <t>Speaker(s)</t>
   </si>
   <si>
     <t>Contact Info</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b val="1"/>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica Neue"/>
-      </rPr>
-      <t>Ben Michel</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica Neue"/>
-      </rPr>
-      <t xml:space="preserve"> - Open Discussion on Topics for the Year</t>
-    </r>
+    <t>Speaker</t>
   </si>
   <si>
     <r>
@@ -51,7 +35,7 @@
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
       </rPr>
-      <t>Andrew Chalkley</t>
+      <t>Ben Michel</t>
     </r>
     <r>
       <rPr>
@@ -59,12 +43,121 @@
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
       </rPr>
-      <t xml:space="preserve"> - his new edition of the JavaScript of Things SDK.</t>
+      <t xml:space="preserve"> - Open Discussion on Topics for the Year</t>
     </r>
   </si>
   <si>
     <r>
       <rPr>
+        <b val="1"/>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>Lightning Talk Alchemy Code Lab Students, Twitter Bot “Markov Twain”</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t xml:space="preserve">: Jodi 'JBJ' Kansagor, Brittany Houtz, Jacob Harrington, Joseph Tatum, Joel Durham.
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="12"/>
+        <color indexed="16"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>jodinkansagor@gmail.com</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="12"/>
+        <color indexed="16"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>brittany.houtz@gmail.com</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="12"/>
+        <color indexed="16"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>jacobharringtom4@gmail.com</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="12"/>
+        <color indexed="16"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>josephtatum@gmail.com</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>Andrew Chalkley</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t xml:space="preserve"> - his new edition of the JavaScript of Things SDK.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
         <u val="single"/>
         <sz val="12"/>
         <color indexed="8"/>
@@ -147,7 +240,7 @@
       <rPr>
         <u val="single"/>
         <sz val="12"/>
-        <color indexed="13"/>
+        <color indexed="17"/>
         <rFont val="Times"/>
       </rPr>
       <t>https://github.com/chalkers</t>
@@ -162,7 +255,7 @@
     <numFmt numFmtId="0" formatCode="General"/>
     <numFmt numFmtId="59" formatCode="mmmm"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -170,6 +263,11 @@
     </font>
     <font>
       <sz val="12"/>
+      <color indexed="8"/>
+      <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <sz val="13"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
     </font>
@@ -182,7 +280,7 @@
     <font>
       <b val="1"/>
       <sz val="13"/>
-      <color indexed="9"/>
+      <color indexed="12"/>
       <name val="Helvetica Neue"/>
     </font>
     <font>
@@ -194,17 +292,23 @@
     <font>
       <u val="single"/>
       <sz val="12"/>
+      <color indexed="16"/>
+      <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="12"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
     </font>
     <font>
       <u val="single"/>
       <sz val="12"/>
-      <color indexed="13"/>
+      <color indexed="17"/>
       <name val="Times"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -219,42 +323,28 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="11"/>
+        <fgColor indexed="12"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="12"/>
+        <fgColor indexed="14"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="15"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="28">
     <border>
       <left/>
       <right/>
       <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -280,6 +370,190 @@
     </border>
     <border>
       <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="11"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="13"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="13"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="11"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="13"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="11"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="13"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="13"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="13"/>
+      </right>
+      <top style="thin">
+        <color indexed="13"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="13"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="13"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="11"/>
+      </right>
+      <top style="thin">
+        <color indexed="13"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="11"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="13"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="13"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="13"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="13"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="13"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="11"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="11"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color indexed="10"/>
       </right>
@@ -291,16 +565,66 @@
       <left style="thin">
         <color indexed="10"/>
       </left>
+      <right style="thin">
+        <color indexed="13"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="13"/>
+      </left>
       <right/>
       <top/>
-      <bottom/>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="11"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="11"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
       <top/>
-      <bottom/>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -309,59 +633,125 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="59" fontId="3" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="4" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="4" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="59" fontId="4" fillId="4" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="5" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="18" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="19" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="20" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="21" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="5" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="17" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="22" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="23" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="24" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="25" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="26" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="27" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -381,10 +771,14 @@
       <rgbColor rgb="ffff00ff"/>
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="ffaaaaaa"/>
+      <rgbColor rgb="ff0096ff"/>
       <rgbColor rgb="fffefffe"/>
       <rgbColor rgb="ff406091"/>
       <rgbColor rgb="ff0075ba"/>
       <rgbColor rgb="ffefeeee"/>
+      <rgbColor rgb="ff0000ff"/>
       <rgbColor rgb="ff0000ee"/>
     </indexedColors>
   </colors>
@@ -402,10 +796,10 @@
         <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="5E5E5E"/>
+        <a:srgbClr val="A7A7A7"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="D5D5D5"/>
+        <a:srgbClr val="535353"/>
       </a:lt2>
       <a:accent1>
         <a:srgbClr val="00A2FF"/>
@@ -582,11 +976,14 @@
     <a:spDef>
       <a:spPr>
         <a:solidFill>
-          <a:schemeClr val="accent1"/>
+          <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="12700" cap="flat">
-          <a:noFill/>
-          <a:miter lim="400000"/>
+        <a:ln w="25400" cap="flat">
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -595,27 +992,27 @@
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="457200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
-          <a:lnSpc>
-            <a:spcPct val="100000"/>
-          </a:lnSpc>
-          <a:spcBef>
-            <a:spcPts val="0"/>
-          </a:spcBef>
-          <a:spcAft>
-            <a:spcPts val="0"/>
-          </a:spcAft>
-          <a:buClrTx/>
-          <a:buSzTx/>
-          <a:buFontTx/>
-          <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1200" u="none" kumimoji="0" normalizeH="0">
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:solidFill>
-              <a:srgbClr val="FFFFFF"/>
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
@@ -872,10 +1269,10 @@
         <a:noFill/>
         <a:ln w="25400" cap="flat">
           <a:solidFill>
-            <a:srgbClr val="000000"/>
+            <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="400000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -1166,7 +1563,7 @@
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="457200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
           <a:lnSpc>
             <a:spcPct val="100000"/>
           </a:lnSpc>
@@ -1444,18 +1841,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A2:K16"/>
+  <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
-      <pane topLeftCell="B3" xSplit="1" ySplit="2" activePane="bottomRight" state="frozen"/>
-    </sheetView>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="16.3516" style="1" customWidth="1"/>
-    <col min="2" max="2" width="26.6719" style="1" customWidth="1"/>
-    <col min="3" max="3" width="26.6328" style="1" customWidth="1"/>
-    <col min="4" max="9" width="26.6719" style="1" customWidth="1"/>
+    <col min="2" max="9" width="26.6719" style="1" customWidth="1"/>
     <col min="10" max="11" width="16.3516" style="1" customWidth="1"/>
     <col min="12" max="256" width="16.3516" style="1" customWidth="1"/>
   </cols>
@@ -1464,274 +1857,279 @@
       <c r="A1" t="s" s="2">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="5"/>
     </row>
     <row r="2" ht="24.1" customHeight="1">
-      <c r="A2" t="s" s="3">
+      <c r="A2" t="s" s="6">
         <v>1</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="5">
+      <c r="B2" s="7"/>
+      <c r="C2" s="8">
         <v>2020</v>
       </c>
-      <c r="D2" s="4"/>
-      <c r="E2" s="5">
+      <c r="D2" s="9"/>
+      <c r="E2" s="10">
         <v>2021</v>
       </c>
-      <c r="F2" s="4"/>
-      <c r="G2" s="5">
+      <c r="F2" s="7"/>
+      <c r="G2" s="10">
         <v>2022</v>
       </c>
-      <c r="H2" s="4"/>
-      <c r="I2" s="5">
+      <c r="H2" s="7"/>
+      <c r="I2" s="10">
         <v>2023</v>
       </c>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="11"/>
     </row>
     <row r="3" ht="24.1" customHeight="1">
-      <c r="A3" s="6"/>
-      <c r="B3" t="s" s="7">
+      <c r="A3" s="12"/>
+      <c r="B3" t="s" s="13">
         <v>2</v>
       </c>
-      <c r="C3" t="s" s="8">
+      <c r="C3" t="s" s="14">
         <v>3</v>
       </c>
-      <c r="D3" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="E3" t="s" s="8">
+      <c r="D3" t="s" s="15">
+        <v>4</v>
+      </c>
+      <c r="E3" t="s" s="16">
         <v>3</v>
       </c>
-      <c r="F3" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="G3" t="s" s="8">
+      <c r="F3" t="s" s="16">
+        <v>4</v>
+      </c>
+      <c r="G3" t="s" s="16">
         <v>3</v>
       </c>
-      <c r="H3" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="I3" t="s" s="8">
+      <c r="H3" t="s" s="16">
+        <v>4</v>
+      </c>
+      <c r="I3" t="s" s="16">
         <v>3</v>
       </c>
-      <c r="J3" s="9"/>
-      <c r="K3" s="9"/>
+      <c r="J3" s="17"/>
+      <c r="K3" s="18"/>
     </row>
     <row r="4" ht="50.65" customHeight="1">
-      <c r="A4" s="10">
+      <c r="A4" s="19">
         <v>43831</v>
       </c>
-      <c r="B4" t="s" s="11">
-        <v>4</v>
-      </c>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="12"/>
-      <c r="K4" s="12"/>
+      <c r="B4" t="s" s="20">
+        <v>5</v>
+      </c>
+      <c r="C4" s="21"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="23"/>
+      <c r="I4" s="23"/>
+      <c r="J4" s="23"/>
+      <c r="K4" s="24"/>
     </row>
-    <row r="5" ht="23.6" customHeight="1">
-      <c r="A5" s="10">
+    <row r="5" ht="118.65" customHeight="1">
+      <c r="A5" s="19">
         <v>43862</v>
       </c>
-      <c r="B5" s="13"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="14"/>
-      <c r="K5" s="14"/>
+      <c r="B5" t="s" s="25">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s" s="26">
+        <v>7</v>
+      </c>
+      <c r="D5" s="27"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="28"/>
+      <c r="G5" s="28"/>
+      <c r="H5" s="28"/>
+      <c r="I5" s="28"/>
+      <c r="J5" s="28"/>
+      <c r="K5" s="29"/>
     </row>
     <row r="6" ht="92" customHeight="1">
-      <c r="A6" s="10">
+      <c r="A6" s="19">
         <v>43891</v>
       </c>
-      <c r="B6" t="s" s="11">
-        <v>5</v>
-      </c>
-      <c r="C6" t="s" s="15">
-        <v>6</v>
-      </c>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="12"/>
+      <c r="B6" t="s" s="20">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s" s="30">
+        <v>9</v>
+      </c>
+      <c r="D6" s="22"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="23"/>
+      <c r="I6" s="23"/>
+      <c r="J6" s="23"/>
+      <c r="K6" s="24"/>
     </row>
     <row r="7" ht="23.6" customHeight="1">
-      <c r="A7" s="10">
+      <c r="A7" s="19">
         <v>43922</v>
       </c>
-      <c r="B7" s="13"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="14"/>
-      <c r="K7" s="14"/>
+      <c r="B7" s="31"/>
+      <c r="C7" s="32"/>
+      <c r="D7" s="27"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="28"/>
+      <c r="G7" s="28"/>
+      <c r="H7" s="28"/>
+      <c r="I7" s="28"/>
+      <c r="J7" s="28"/>
+      <c r="K7" s="29"/>
     </row>
     <row r="8" ht="23.6" customHeight="1">
-      <c r="A8" s="10">
+      <c r="A8" s="19">
         <v>43952</v>
       </c>
-      <c r="B8" s="16"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="12"/>
-      <c r="J8" s="12"/>
-      <c r="K8" s="12"/>
+      <c r="B8" s="33"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="23"/>
+      <c r="H8" s="23"/>
+      <c r="I8" s="23"/>
+      <c r="J8" s="23"/>
+      <c r="K8" s="24"/>
     </row>
     <row r="9" ht="23.6" customHeight="1">
-      <c r="A9" s="10">
+      <c r="A9" s="19">
         <v>43983</v>
       </c>
-      <c r="B9" s="13"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="14"/>
-      <c r="K9" s="14"/>
+      <c r="B9" s="31"/>
+      <c r="C9" s="32"/>
+      <c r="D9" s="27"/>
+      <c r="E9" s="28"/>
+      <c r="F9" s="28"/>
+      <c r="G9" s="28"/>
+      <c r="H9" s="28"/>
+      <c r="I9" s="28"/>
+      <c r="J9" s="28"/>
+      <c r="K9" s="29"/>
     </row>
     <row r="10" ht="23.6" customHeight="1">
-      <c r="A10" s="10">
+      <c r="A10" s="19">
         <v>44013</v>
       </c>
-      <c r="B10" s="16"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="12"/>
-      <c r="K10" s="12"/>
+      <c r="B10" s="33"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
+      <c r="G10" s="23"/>
+      <c r="H10" s="23"/>
+      <c r="I10" s="23"/>
+      <c r="J10" s="23"/>
+      <c r="K10" s="24"/>
     </row>
     <row r="11" ht="23.6" customHeight="1">
-      <c r="A11" s="10">
+      <c r="A11" s="19">
         <v>44044</v>
       </c>
-      <c r="B11" s="13"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="14"/>
-      <c r="K11" s="14"/>
+      <c r="B11" s="31"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="27"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="28"/>
+      <c r="H11" s="28"/>
+      <c r="I11" s="28"/>
+      <c r="J11" s="28"/>
+      <c r="K11" s="29"/>
     </row>
     <row r="12" ht="23.6" customHeight="1">
-      <c r="A12" s="10">
+      <c r="A12" s="19">
         <v>44075</v>
       </c>
-      <c r="B12" s="16"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="12"/>
-      <c r="J12" s="12"/>
-      <c r="K12" s="12"/>
+      <c r="B12" s="33"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="22"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="23"/>
+      <c r="G12" s="23"/>
+      <c r="H12" s="23"/>
+      <c r="I12" s="23"/>
+      <c r="J12" s="23"/>
+      <c r="K12" s="24"/>
     </row>
     <row r="13" ht="23.6" customHeight="1">
-      <c r="A13" s="10">
+      <c r="A13" s="19">
         <v>44105</v>
       </c>
-      <c r="B13" s="13"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="14"/>
-      <c r="K13" s="14"/>
+      <c r="B13" s="31"/>
+      <c r="C13" s="32"/>
+      <c r="D13" s="27"/>
+      <c r="E13" s="28"/>
+      <c r="F13" s="28"/>
+      <c r="G13" s="28"/>
+      <c r="H13" s="28"/>
+      <c r="I13" s="28"/>
+      <c r="J13" s="28"/>
+      <c r="K13" s="29"/>
     </row>
     <row r="14" ht="23.6" customHeight="1">
-      <c r="A14" s="10">
+      <c r="A14" s="19">
         <v>44136</v>
       </c>
-      <c r="B14" s="16"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="12"/>
-      <c r="J14" s="12"/>
-      <c r="K14" s="12"/>
+      <c r="B14" s="33"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="23"/>
+      <c r="F14" s="23"/>
+      <c r="G14" s="23"/>
+      <c r="H14" s="23"/>
+      <c r="I14" s="23"/>
+      <c r="J14" s="23"/>
+      <c r="K14" s="24"/>
     </row>
     <row r="15" ht="23.6" customHeight="1">
-      <c r="A15" s="10">
+      <c r="A15" s="19">
         <v>44166</v>
       </c>
-      <c r="B15" s="13"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
-      <c r="K15" s="14"/>
+      <c r="B15" s="31"/>
+      <c r="C15" s="32"/>
+      <c r="D15" s="27"/>
+      <c r="E15" s="28"/>
+      <c r="F15" s="28"/>
+      <c r="G15" s="28"/>
+      <c r="H15" s="28"/>
+      <c r="I15" s="28"/>
+      <c r="J15" s="28"/>
+      <c r="K15" s="29"/>
     </row>
     <row r="16" ht="23.6" customHeight="1">
-      <c r="A16" s="17"/>
-      <c r="B16" s="16"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="12"/>
-      <c r="I16" s="12"/>
-      <c r="J16" s="12"/>
-      <c r="K16" s="12"/>
+      <c r="A16" s="34"/>
+      <c r="B16" s="35"/>
+      <c r="C16" s="36"/>
+      <c r="D16" s="37"/>
+      <c r="E16" s="38"/>
+      <c r="F16" s="38"/>
+      <c r="G16" s="38"/>
+      <c r="H16" s="38"/>
+      <c r="I16" s="38"/>
+      <c r="J16" s="38"/>
+      <c r="K16" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:K1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="C6" r:id="rId1" location="" tooltip="" display="andrew@chalkley.org"/>
+    <hyperlink ref="C5" r:id="rId1" location="" tooltip="" display="jodinkansagor@gmail.com"/>
+    <hyperlink ref="C6" r:id="rId2" location="" tooltip="" display="andrew@chalkley.org&#10;(407) 923-4889&#10;@chalkers on Twitter&#10;https://jsot.slack.com&#10;http://andrew.chalkley.org/&#10;https://github.com/chalkers"/>
   </hyperlinks>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="72" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>

</xml_diff>